<commit_message>
Deep Audit complete: Removed all hardcoded defaults + added verify_integrity_suite.py
</commit_message>
<xml_diff>
--- a/CFO Dashboard/Finance_Dashboard_Final.xlsx
+++ b/CFO Dashboard/Finance_Dashboard_Final.xlsx
@@ -731,28 +731,28 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -793,28 +793,28 @@
         </is>
       </c>
       <c r="B19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -824,28 +824,28 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1293,10 +1293,10 @@
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="17" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0</v>
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="17" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="17" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Final Dashboard Enhancements: Visuals, Fixes, and Integrity Suite
</commit_message>
<xml_diff>
--- a/CFO Dashboard/Finance_Dashboard_Final.xlsx
+++ b/CFO Dashboard/Finance_Dashboard_Final.xlsx
@@ -137,7 +137,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -151,6 +151,26 @@
         <patternFill patternType="solid">
           <fgColor rgb="00C6EFCE"/>
           <bgColor rgb="00C6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="00C00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="0000B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFEB84"/>
+          <bgColor rgb="00FFEB84"/>
         </patternFill>
       </fill>
     </dxf>
@@ -225,6 +245,306 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="12"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Liquidity Forecast (Cash Balance)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Ending Cash</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'LIQUIDITY_MONITOR'!$B$14:$I$14</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'LIQUIDITY_MONITOR'!$B$30:$I$30</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Fortnight</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cash Balance ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Solvency Gauge (Debt Ratio)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'BALANCE_SHEET_HEALTH'!I12</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'BALANCE_SHEET_HEALTH'!$H$13:$H$14</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'BALANCE_SHEET_HEALTH'!$I$13:$I$14</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'BALANCE_SHEET_HEALTH'!J12</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln w="20000">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'BALANCE_SHEET_HEALTH'!$J$13:$J$14</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="200"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+      <valAx>
+        <axId val="200"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3600000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1113,6 +1433,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1348,11 +1669,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" priority="1" dxfId="0">
+    <cfRule type="expression" priority="1" dxfId="2">
       <formula>C17&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" priority="2" dxfId="1">
+    <cfRule type="expression" priority="2" dxfId="3">
       <formula>C17&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D17">
+    <cfRule type="expression" priority="3" dxfId="4">
+      <formula>ABS(D12)&gt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1365,7 +1691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,6 +1764,23 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Ratio</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Limit</t>
+        </is>
+      </c>
+    </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
@@ -1448,6 +1791,32 @@
         <f>B6/B5</f>
         <v/>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="I13">
+        <f>B13</f>
+        <v/>
+      </c>
+      <c r="J13" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Post-Decision</t>
+        </is>
+      </c>
+      <c r="I14">
+        <f>B19</f>
+        <v/>
+      </c>
+      <c r="J14" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1510,11 +1879,6 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>Equity Check</t>
-        </is>
-      </c>
       <c r="B23" s="15">
         <f>IF(B8&lt;0,"CRITICAL: Equity Erosion. Retained earnings negative.","Equity OK")</f>
         <v/>
@@ -1522,6 +1886,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Backup: Save all current work including dashboard generations and README updates
</commit_message>
<xml_diff>
--- a/CFO Dashboard/Finance_Dashboard_Final.xlsx
+++ b/CFO Dashboard/Finance_Dashboard_Final.xlsx
@@ -24,7 +24,7 @@
     <numFmt numFmtId="164" formatCode="$#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -46,15 +46,18 @@
       <b val="1"/>
     </font>
     <font>
+      <i val="1"/>
+      <color rgb="00666666"/>
+    </font>
+    <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
     <font>
       <i val="1"/>
-      <color rgb="00666666"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -75,8 +78,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
+        <fgColor rgb="00B4B4B4"/>
+        <bgColor rgb="00B4B4B4"/>
       </patternFill>
     </fill>
     <fill>
@@ -89,6 +92,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00E2EFDA"/>
         <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -110,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -119,20 +128,24 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -295,7 +308,7 @@
           </cat>
           <val>
             <numRef>
-              <f>'LIQUIDITY_MONITOR'!$B$30:$I$30</f>
+              <f>'LIQUIDITY_MONITOR'!$B$33:$I$33</f>
             </numRef>
           </val>
         </ser>
@@ -836,7 +849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,7 +889,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>555000</v>
+        <v>134500</v>
       </c>
     </row>
     <row r="6">
@@ -886,7 +899,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>75000</v>
+        <v>32749</v>
       </c>
     </row>
     <row r="7">
@@ -912,12 +925,16 @@
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>STARTING CASH FOR FN1</t>
-        </is>
-      </c>
-      <c r="B9" s="7">
-        <f>B5-B6-B7-B8</f>
-        <v/>
+          <t>STARTING CASH FOR FN1 (HARD)</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>134500</v>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
+        <is>
+          <t>← From initial_cash_flow.xlsx</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -928,47 +945,47 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="9" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>FN1</t>
         </is>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>FN2</t>
         </is>
       </c>
-      <c r="D14" s="9" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>FN3</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E14" s="10" t="inlineStr">
         <is>
           <t>FN4</t>
         </is>
       </c>
-      <c r="F14" s="9" t="inlineStr">
+      <c r="F14" s="10" t="inlineStr">
         <is>
           <t>FN5</t>
         </is>
       </c>
-      <c r="G14" s="9" t="inlineStr">
+      <c r="G14" s="10" t="inlineStr">
         <is>
           <t>FN6</t>
         </is>
       </c>
-      <c r="H14" s="9" t="inlineStr">
+      <c r="H14" s="10" t="inlineStr">
         <is>
           <t>FN7</t>
         </is>
       </c>
-      <c r="I14" s="9" t="inlineStr">
+      <c r="I14" s="10" t="inlineStr">
         <is>
           <t>FN8</t>
         </is>
@@ -985,31 +1002,31 @@
         <v/>
       </c>
       <c r="C15" s="4">
-        <f>B$30</f>
+        <f>B$33</f>
         <v/>
       </c>
       <c r="D15" s="4">
-        <f>C$30</f>
+        <f>C$33</f>
         <v/>
       </c>
       <c r="E15" s="4">
-        <f>D$30</f>
+        <f>D$33</f>
         <v/>
       </c>
       <c r="F15" s="4">
-        <f>E$30</f>
+        <f>E$33</f>
         <v/>
       </c>
       <c r="G15" s="4">
-        <f>F$30</f>
+        <f>F$33</f>
         <v/>
       </c>
       <c r="H15" s="4">
-        <f>G$30</f>
+        <f>G$33</f>
         <v/>
       </c>
       <c r="I15" s="4">
-        <f>H$30</f>
+        <f>H$33</f>
         <v/>
       </c>
     </row>
@@ -1082,84 +1099,84 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>5250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Receivables (Hard)</t>
+          <t>Receivables (HARD)</t>
         </is>
       </c>
       <c r="B19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="4" t="n">
-        <v>0</v>
+      <c r="C19" s="11" t="n">
+        <v>221338</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="4" t="n">
-        <v>0</v>
+      <c r="E19" s="11" t="n">
+        <v>74219</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="4" t="n">
-        <v>0</v>
+      <c r="G19" s="11" t="n">
+        <v>254176</v>
       </c>
       <c r="H19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="4" t="n">
-        <v>0</v>
+      <c r="I19" s="11" t="n">
+        <v>202017</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Payables (Hard)</t>
+          <t>Payables (HARD)</t>
         </is>
       </c>
       <c r="B20" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>0</v>
+      <c r="C20" s="11" t="n">
+        <v>-94059</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>-15792</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4" t="n">
-        <v>0</v>
+      <c r="F20" s="11" t="n">
+        <v>-46165</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>-69087</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>0</v>
@@ -1168,268 +1185,317 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>SECTION C: FINANCING DECISIONS</t>
         </is>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>Change in Credit Line (+/-)</t>
-        </is>
-      </c>
-      <c r="B23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
-        <is>
-          <t>Change in Investments (+/-)</t>
-        </is>
-      </c>
-      <c r="B24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5" t="n">
-        <v>0</v>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>DEBT CAPACITY (Short Term)</t>
+        </is>
+      </c>
+      <c r="D24" s="12" t="inlineStr">
+        <is>
+          <t>Limit: $500,000</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
+          <t>Change in Credit Line (+/-)</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="inlineStr">
+        <is>
+          <t>Proj. ST Debt Balance</t>
+        </is>
+      </c>
+      <c r="B26" s="13">
+        <f>0+B25</f>
+        <v/>
+      </c>
+      <c r="C26" s="13">
+        <f>B26+C25</f>
+        <v/>
+      </c>
+      <c r="D26" s="13">
+        <f>C26+D25</f>
+        <v/>
+      </c>
+      <c r="E26" s="13">
+        <f>D26+E25</f>
+        <v/>
+      </c>
+      <c r="F26" s="13">
+        <f>E26+F25</f>
+        <v/>
+      </c>
+      <c r="G26" s="13">
+        <f>F26+G25</f>
+        <v/>
+      </c>
+      <c r="H26" s="13">
+        <f>G26+H25</f>
+        <v/>
+      </c>
+      <c r="I26" s="13">
+        <f>H26+I25</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>Change in Investments (+/-)</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
           <t>New Mortgage Inflow</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="inlineStr">
-        <is>
-          <t>Dividends Paid</t>
-        </is>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>SECTION D: CASH BALANCE</t>
-        </is>
+      <c r="B28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
+          <t>Dividends Paid</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>SECTION D: CASH BALANCE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
           <t>Net Cash Flow</t>
         </is>
       </c>
-      <c r="B29" s="10">
-        <f>B16+B19+B23+B25-B17-B18-B20-B24-B26</f>
-        <v/>
-      </c>
-      <c r="C29" s="10">
-        <f>C16+C19+C23+C25-C17-C18-C20-C24-C26</f>
-        <v/>
-      </c>
-      <c r="D29" s="10">
-        <f>D16+D19+D23+D25-D17-D18-D20-D24-D26</f>
-        <v/>
-      </c>
-      <c r="E29" s="10">
-        <f>E16+E19+E23+E25-E17-E18-E20-E24-E26</f>
-        <v/>
-      </c>
-      <c r="F29" s="10">
-        <f>F16+F19+F23+F25-F17-F18-F20-F24-F26</f>
-        <v/>
-      </c>
-      <c r="G29" s="10">
-        <f>G16+G19+G23+G25-G17-G18-G20-G24-G26</f>
-        <v/>
-      </c>
-      <c r="H29" s="10">
-        <f>H16+H19+H23+H25-H17-H18-H20-H24-H26</f>
-        <v/>
-      </c>
-      <c r="I29" s="10">
-        <f>I16+I19+I23+I25-I17-I18-I20-I24-I26</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="inlineStr">
+      <c r="B32" s="14">
+        <f>B16+B19+B25+B28-B17-B18-B20-B27-B29</f>
+        <v/>
+      </c>
+      <c r="C32" s="14">
+        <f>C16+C19+C25+C28-C17-C18-C20-C27-C29</f>
+        <v/>
+      </c>
+      <c r="D32" s="14">
+        <f>D16+D19+D25+D28-D17-D18-D20-D27-D29</f>
+        <v/>
+      </c>
+      <c r="E32" s="14">
+        <f>E16+E19+E25+E28-E17-E18-E20-E27-E29</f>
+        <v/>
+      </c>
+      <c r="F32" s="14">
+        <f>F16+F19+F25+F28-F17-F18-F20-F27-F29</f>
+        <v/>
+      </c>
+      <c r="G32" s="14">
+        <f>G16+G19+G25+G28-G17-G18-G20-G27-G29</f>
+        <v/>
+      </c>
+      <c r="H32" s="14">
+        <f>H16+H19+H25+H28-H17-H18-H20-H27-H29</f>
+        <v/>
+      </c>
+      <c r="I32" s="14">
+        <f>I16+I19+I25+I28-I17-I18-I20-I27-I29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
         <is>
           <t>ENDING CASH BALANCE</t>
         </is>
       </c>
-      <c r="B30" s="7">
-        <f>B15+B29</f>
-        <v/>
-      </c>
-      <c r="C30" s="7">
-        <f>C15+C29</f>
-        <v/>
-      </c>
-      <c r="D30" s="7">
-        <f>D15+D29</f>
-        <v/>
-      </c>
-      <c r="E30" s="7">
-        <f>E15+E29</f>
-        <v/>
-      </c>
-      <c r="F30" s="7">
-        <f>F15+F29</f>
-        <v/>
-      </c>
-      <c r="G30" s="7">
-        <f>G15+G29</f>
-        <v/>
-      </c>
-      <c r="H30" s="7">
-        <f>H15+H29</f>
-        <v/>
-      </c>
-      <c r="I30" s="7">
-        <f>I15+I29</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="inlineStr">
+      <c r="B33" s="15">
+        <f>B15+B32</f>
+        <v/>
+      </c>
+      <c r="C33" s="15">
+        <f>C15+C32</f>
+        <v/>
+      </c>
+      <c r="D33" s="15">
+        <f>D15+D32</f>
+        <v/>
+      </c>
+      <c r="E33" s="15">
+        <f>E15+E32</f>
+        <v/>
+      </c>
+      <c r="F33" s="15">
+        <f>F15+F32</f>
+        <v/>
+      </c>
+      <c r="G33" s="15">
+        <f>G15+G32</f>
+        <v/>
+      </c>
+      <c r="H33" s="15">
+        <f>H15+H32</f>
+        <v/>
+      </c>
+      <c r="I33" s="15">
+        <f>I15+I32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>Solvency Check</t>
         </is>
       </c>
-      <c r="B31" s="3">
-        <f>IF(B30&lt;0,"INSOLVENT!",IF(B30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="C31" s="3">
-        <f>IF(C30&lt;0,"INSOLVENT!",IF(C30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="D31" s="3">
-        <f>IF(D30&lt;0,"INSOLVENT!",IF(D30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="E31" s="3">
-        <f>IF(E30&lt;0,"INSOLVENT!",IF(E30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="F31" s="3">
-        <f>IF(F30&lt;0,"INSOLVENT!",IF(F30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="G31" s="3">
-        <f>IF(G30&lt;0,"INSOLVENT!",IF(G30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="H31" s="3">
-        <f>IF(H30&lt;0,"INSOLVENT!",IF(H30&gt;200000,"Excess Cash","OK"))</f>
-        <v/>
-      </c>
-      <c r="I31" s="3">
-        <f>IF(I30&lt;0,"INSOLVENT!",IF(I30&gt;200000,"Excess Cash","OK"))</f>
+      <c r="B34" s="3">
+        <f>IF(B33&lt;0,"INSOLVENT!",IF(B33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="C34" s="3">
+        <f>IF(C33&lt;0,"INSOLVENT!",IF(C33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="D34" s="3">
+        <f>IF(D33&lt;0,"INSOLVENT!",IF(D33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="E34" s="3">
+        <f>IF(E33&lt;0,"INSOLVENT!",IF(E33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="F34" s="3">
+        <f>IF(F33&lt;0,"INSOLVENT!",IF(F33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="G34" s="3">
+        <f>IF(G33&lt;0,"INSOLVENT!",IF(G33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="H34" s="3">
+        <f>IF(H33&lt;0,"INSOLVENT!",IF(H33&gt;200000,"Excess Cash","OK"))</f>
+        <v/>
+      </c>
+      <c r="I34" s="3">
+        <f>IF(I33&lt;0,"INSOLVENT!",IF(I33&gt;200000,"Excess Cash","OK"))</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B30:I30">
+  <conditionalFormatting sqref="B33:I33">
     <cfRule type="expression" priority="1" dxfId="0">
-      <formula>B30&lt;0</formula>
+      <formula>B33&lt;0</formula>
     </cfRule>
     <cfRule type="expression" priority="2" dxfId="1">
-      <formula>B30&gt;200000</formula>
+      <formula>B33&gt;200000</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1443,7 +1509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1477,8 +1543,8 @@
           <t>Historical Gross Margin %</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n">
-        <v>0.4</v>
+      <c r="B5" s="16" t="n">
+        <v>0.5911697410270922</v>
       </c>
     </row>
     <row r="6">
@@ -1487,8 +1553,8 @@
           <t>Historical Net Margin %</t>
         </is>
       </c>
-      <c r="B6" s="11" t="n">
-        <v>0.1358</v>
+      <c r="B6" s="16" t="n">
+        <v>0.03904386988246832</v>
       </c>
     </row>
     <row r="9">
@@ -1499,22 +1565,22 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="inlineStr">
+      <c r="A10" s="17" t="inlineStr">
         <is>
           <t>Line Item</t>
         </is>
       </c>
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>Last Round Actuals</t>
         </is>
       </c>
-      <c r="C10" s="12" t="inlineStr">
+      <c r="C10" s="17" t="inlineStr">
         <is>
           <t>This Round Projected</t>
         </is>
       </c>
-      <c r="D10" s="12" t="inlineStr">
+      <c r="D10" s="17" t="inlineStr">
         <is>
           <t>Variance %</t>
         </is>
@@ -1527,12 +1593,12 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>2500000</v>
+        <v>952339</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>2500000</v>
-      </c>
-      <c r="D11" s="13">
+        <v>952339</v>
+      </c>
+      <c r="D11" s="18">
         <f>IF(B11&gt;0,(C11-B11)/B11,0)</f>
         <v/>
       </c>
@@ -1544,13 +1610,13 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="C12" s="10">
+        <v>389345</v>
+      </c>
+      <c r="C12" s="14">
         <f>C11*(1-$B$5)</f>
         <v/>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="18">
         <f>IF(B12&gt;0,(C12-B12)/B12,0)</f>
         <v/>
       </c>
@@ -1562,13 +1628,13 @@
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C13" s="10">
+        <v>562994</v>
+      </c>
+      <c r="C13" s="14">
         <f>C11-C12</f>
         <v/>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="18">
         <f>IF(B13&gt;0,(C13-B13)/B13,0)</f>
         <v/>
       </c>
@@ -1580,12 +1646,12 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>42000</v>
+        <v>0</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>42000</v>
-      </c>
-      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18">
         <f>IF(B14&gt;0,(C14-B14)/B14,0)</f>
         <v/>
       </c>
@@ -1593,18 +1659,23 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Depreciation</t>
+          <t>Depreciation (HARD)</t>
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>120000</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>120000</v>
-      </c>
-      <c r="D15" s="13">
+        <v>409407</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>28960</v>
+      </c>
+      <c r="D15" s="18">
         <f>IF(B15&gt;0,(C15-B15)/B15,0)</f>
         <v/>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>← Auto-calc from machine_spaces.xlsx</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1626,14 +1697,14 @@
           <t>EST. NET INCOME</t>
         </is>
       </c>
-      <c r="B17" s="14" t="n">
-        <v>339500</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="19" t="n">
+        <v>37183</v>
+      </c>
+      <c r="C17" s="15">
         <f>C13-C14-C15-C16</f>
         <v/>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="18">
         <f>IF(B17&gt;0,(C17-B17)/B17,0)</f>
         <v/>
       </c>
@@ -1651,7 +1722,7 @@
           <t>Projected Net Margin</t>
         </is>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="18">
         <f>IF(C11&gt;0,C17/C11,0)</f>
         <v/>
       </c>
@@ -1662,7 +1733,7 @@
           <t>Profit Realism Flag</t>
         </is>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="20">
         <f>IF(B20&gt;$B$6+0.05,"WARNING: Unrealistic profit jump!","Projection OK")</f>
         <v/>
       </c>
@@ -1724,7 +1795,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>4200000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1734,7 +1805,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1680000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1744,7 +1815,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>2520000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1754,7 +1825,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>850000</v>
+        <v>181621</v>
       </c>
     </row>
     <row r="11">
@@ -1787,7 +1858,7 @@
           <t>Current Debt Ratio</t>
         </is>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="18">
         <f>B6/B5</f>
         <v/>
       </c>
@@ -1844,7 +1915,7 @@
           <t>Total New Debt</t>
         </is>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="14">
         <f>B15+B16</f>
         <v/>
       </c>
@@ -1855,7 +1926,7 @@
           <t>Est. Post-Decision Debt Ratio</t>
         </is>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="21">
         <f>(B6+B17)/B5</f>
         <v/>
       </c>
@@ -1873,13 +1944,13 @@
           <t>Debt Level Check</t>
         </is>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="20">
         <f>IF(B19&gt;0.6,"CRITICAL: Debt too high. Credit Rating Risk.","Health OK")</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="15">
+      <c r="B23" s="20">
         <f>IF(B8&lt;0,"CRITICAL: Equity Erosion. Retained earnings negative.","Equity OK")</f>
         <v/>
       </c>
@@ -1896,7 +1967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1927,32 +1998,32 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="17" t="inlineStr">
         <is>
           <t>Loan #</t>
         </is>
       </c>
-      <c r="B5" s="12" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="C5" s="12" t="inlineStr">
+      <c r="C5" s="17" t="inlineStr">
         <is>
           <t>Interest Rate</t>
         </is>
       </c>
-      <c r="D5" s="12" t="inlineStr">
+      <c r="D5" s="17" t="inlineStr">
         <is>
           <t>Payment Period 1</t>
         </is>
       </c>
-      <c r="E5" s="12" t="inlineStr">
+      <c r="E5" s="17" t="inlineStr">
         <is>
           <t>Payment Period 2</t>
         </is>
       </c>
-      <c r="F5" s="12" t="inlineStr">
+      <c r="F5" s="17" t="inlineStr">
         <is>
           <t>Total Payments</t>
         </is>
@@ -1967,7 +2038,7 @@
       <c r="B6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="17" t="n">
+      <c r="C6" s="22" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="5" t="n">
@@ -1976,7 +2047,7 @@
       <c r="E6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="14">
         <f>D6+E6</f>
         <v/>
       </c>
@@ -1990,7 +2061,7 @@
       <c r="B7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="17" t="n">
+      <c r="C7" s="22" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="5" t="n">
@@ -1999,7 +2070,7 @@
       <c r="E7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="14">
         <f>D7+E7</f>
         <v/>
       </c>
@@ -2013,7 +2084,7 @@
       <c r="B8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="17" t="n">
+      <c r="C8" s="22" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="5" t="n">
@@ -2022,7 +2093,7 @@
       <c r="E8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="14">
         <f>D8+E8</f>
         <v/>
       </c>
@@ -2033,16 +2104,64 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="23">
         <f>SUM(B6:B8)</f>
         <v/>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="23">
         <f>SUM(F6:F8)</f>
         <v/>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>DIVIDEND CONTROL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Max Dividend Capacity (HARD)</t>
+        </is>
+      </c>
+      <c r="B14" s="11" t="n">
+        <v>181621</v>
+      </c>
+      <c r="C14" s="8" t="inlineStr">
+        <is>
+          <t>← Retained Earnings from balance sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>User Dividend Input</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Dividend Status</t>
+        </is>
+      </c>
+      <c r="B16" s="3">
+        <f>IF(B15&gt;B14,"❌ ILLEGAL: Exceeds Retained Earnings","✓ LEGAL")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>$B$15&gt;$B$14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2080,7 +2199,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Copy these values to ExSim Finance upload</t>
         </is>
@@ -2094,42 +2213,42 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="12" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>FN1</t>
         </is>
       </c>
-      <c r="C5" s="12" t="inlineStr">
+      <c r="C5" s="17" t="inlineStr">
         <is>
           <t>FN2</t>
         </is>
       </c>
-      <c r="D5" s="12" t="inlineStr">
+      <c r="D5" s="17" t="inlineStr">
         <is>
           <t>FN3</t>
         </is>
       </c>
-      <c r="E5" s="12" t="inlineStr">
+      <c r="E5" s="17" t="inlineStr">
         <is>
           <t>FN4</t>
         </is>
       </c>
-      <c r="F5" s="12" t="inlineStr">
+      <c r="F5" s="17" t="inlineStr">
         <is>
           <t>FN5</t>
         </is>
       </c>
-      <c r="G5" s="12" t="inlineStr">
+      <c r="G5" s="17" t="inlineStr">
         <is>
           <t>FN6</t>
         </is>
       </c>
-      <c r="H5" s="12" t="inlineStr">
+      <c r="H5" s="17" t="inlineStr">
         <is>
           <t>FN7</t>
         </is>
       </c>
-      <c r="I5" s="12" t="inlineStr">
+      <c r="I5" s="17" t="inlineStr">
         <is>
           <t>FN8</t>
         </is>
@@ -2141,36 +2260,36 @@
           <t>Amount</t>
         </is>
       </c>
-      <c r="B6" s="10">
-        <f>LIQUIDITY_MONITOR!B23</f>
-        <v/>
-      </c>
-      <c r="C6" s="10">
-        <f>LIQUIDITY_MONITOR!C23</f>
-        <v/>
-      </c>
-      <c r="D6" s="10">
-        <f>LIQUIDITY_MONITOR!D23</f>
-        <v/>
-      </c>
-      <c r="E6" s="10">
-        <f>LIQUIDITY_MONITOR!E23</f>
-        <v/>
-      </c>
-      <c r="F6" s="10">
-        <f>LIQUIDITY_MONITOR!F23</f>
-        <v/>
-      </c>
-      <c r="G6" s="10">
-        <f>LIQUIDITY_MONITOR!G23</f>
-        <v/>
-      </c>
-      <c r="H6" s="10">
-        <f>LIQUIDITY_MONITOR!H23</f>
-        <v/>
-      </c>
-      <c r="I6" s="10">
-        <f>LIQUIDITY_MONITOR!I23</f>
+      <c r="B6" s="14">
+        <f>LIQUIDITY_MONITOR!B25</f>
+        <v/>
+      </c>
+      <c r="C6" s="14">
+        <f>LIQUIDITY_MONITOR!C25</f>
+        <v/>
+      </c>
+      <c r="D6" s="14">
+        <f>LIQUIDITY_MONITOR!D25</f>
+        <v/>
+      </c>
+      <c r="E6" s="14">
+        <f>LIQUIDITY_MONITOR!E25</f>
+        <v/>
+      </c>
+      <c r="F6" s="14">
+        <f>LIQUIDITY_MONITOR!F25</f>
+        <v/>
+      </c>
+      <c r="G6" s="14">
+        <f>LIQUIDITY_MONITOR!G25</f>
+        <v/>
+      </c>
+      <c r="H6" s="14">
+        <f>LIQUIDITY_MONITOR!H25</f>
+        <v/>
+      </c>
+      <c r="I6" s="14">
+        <f>LIQUIDITY_MONITOR!I25</f>
         <v/>
       </c>
     </row>
@@ -2182,42 +2301,42 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>FN1</t>
         </is>
       </c>
-      <c r="C10" s="12" t="inlineStr">
+      <c r="C10" s="17" t="inlineStr">
         <is>
           <t>FN2</t>
         </is>
       </c>
-      <c r="D10" s="12" t="inlineStr">
+      <c r="D10" s="17" t="inlineStr">
         <is>
           <t>FN3</t>
         </is>
       </c>
-      <c r="E10" s="12" t="inlineStr">
+      <c r="E10" s="17" t="inlineStr">
         <is>
           <t>FN4</t>
         </is>
       </c>
-      <c r="F10" s="12" t="inlineStr">
+      <c r="F10" s="17" t="inlineStr">
         <is>
           <t>FN5</t>
         </is>
       </c>
-      <c r="G10" s="12" t="inlineStr">
+      <c r="G10" s="17" t="inlineStr">
         <is>
           <t>FN6</t>
         </is>
       </c>
-      <c r="H10" s="12" t="inlineStr">
+      <c r="H10" s="17" t="inlineStr">
         <is>
           <t>FN7</t>
         </is>
       </c>
-      <c r="I10" s="12" t="inlineStr">
+      <c r="I10" s="17" t="inlineStr">
         <is>
           <t>FN8</t>
         </is>
@@ -2229,36 +2348,36 @@
           <t>Amount</t>
         </is>
       </c>
-      <c r="B11" s="10">
-        <f>LIQUIDITY_MONITOR!B24</f>
-        <v/>
-      </c>
-      <c r="C11" s="10">
-        <f>LIQUIDITY_MONITOR!C24</f>
-        <v/>
-      </c>
-      <c r="D11" s="10">
-        <f>LIQUIDITY_MONITOR!D24</f>
-        <v/>
-      </c>
-      <c r="E11" s="10">
-        <f>LIQUIDITY_MONITOR!E24</f>
-        <v/>
-      </c>
-      <c r="F11" s="10">
-        <f>LIQUIDITY_MONITOR!F24</f>
-        <v/>
-      </c>
-      <c r="G11" s="10">
-        <f>LIQUIDITY_MONITOR!G24</f>
-        <v/>
-      </c>
-      <c r="H11" s="10">
-        <f>LIQUIDITY_MONITOR!H24</f>
-        <v/>
-      </c>
-      <c r="I11" s="10">
-        <f>LIQUIDITY_MONITOR!I24</f>
+      <c r="B11" s="14">
+        <f>LIQUIDITY_MONITOR!B27</f>
+        <v/>
+      </c>
+      <c r="C11" s="14">
+        <f>LIQUIDITY_MONITOR!C27</f>
+        <v/>
+      </c>
+      <c r="D11" s="14">
+        <f>LIQUIDITY_MONITOR!D27</f>
+        <v/>
+      </c>
+      <c r="E11" s="14">
+        <f>LIQUIDITY_MONITOR!E27</f>
+        <v/>
+      </c>
+      <c r="F11" s="14">
+        <f>LIQUIDITY_MONITOR!F27</f>
+        <v/>
+      </c>
+      <c r="G11" s="14">
+        <f>LIQUIDITY_MONITOR!G27</f>
+        <v/>
+      </c>
+      <c r="H11" s="14">
+        <f>LIQUIDITY_MONITOR!H27</f>
+        <v/>
+      </c>
+      <c r="I11" s="14">
+        <f>LIQUIDITY_MONITOR!I27</f>
         <v/>
       </c>
     </row>
@@ -2270,22 +2389,22 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="inlineStr">
+      <c r="A15" s="17" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="B15" s="12" t="inlineStr">
+      <c r="B15" s="17" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="C15" s="12" t="inlineStr">
+      <c r="C15" s="17" t="inlineStr">
         <is>
           <t>Payment 1</t>
         </is>
       </c>
-      <c r="D15" s="12" t="inlineStr">
+      <c r="D15" s="17" t="inlineStr">
         <is>
           <t>Payment 2</t>
         </is>
@@ -2356,36 +2475,36 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="10">
-        <f>LIQUIDITY_MONITOR!B26</f>
-        <v/>
-      </c>
-      <c r="C22" s="10">
-        <f>LIQUIDITY_MONITOR!C26</f>
-        <v/>
-      </c>
-      <c r="D22" s="10">
-        <f>LIQUIDITY_MONITOR!D26</f>
-        <v/>
-      </c>
-      <c r="E22" s="10">
-        <f>LIQUIDITY_MONITOR!E26</f>
-        <v/>
-      </c>
-      <c r="F22" s="10">
-        <f>LIQUIDITY_MONITOR!F26</f>
-        <v/>
-      </c>
-      <c r="G22" s="10">
-        <f>LIQUIDITY_MONITOR!G26</f>
-        <v/>
-      </c>
-      <c r="H22" s="10">
-        <f>LIQUIDITY_MONITOR!H26</f>
-        <v/>
-      </c>
-      <c r="I22" s="10">
-        <f>LIQUIDITY_MONITOR!I26</f>
+      <c r="B22" s="14">
+        <f>LIQUIDITY_MONITOR!B29</f>
+        <v/>
+      </c>
+      <c r="C22" s="14">
+        <f>LIQUIDITY_MONITOR!C29</f>
+        <v/>
+      </c>
+      <c r="D22" s="14">
+        <f>LIQUIDITY_MONITOR!D29</f>
+        <v/>
+      </c>
+      <c r="E22" s="14">
+        <f>LIQUIDITY_MONITOR!E29</f>
+        <v/>
+      </c>
+      <c r="F22" s="14">
+        <f>LIQUIDITY_MONITOR!F29</f>
+        <v/>
+      </c>
+      <c r="G22" s="14">
+        <f>LIQUIDITY_MONITOR!G29</f>
+        <v/>
+      </c>
+      <c r="H22" s="14">
+        <f>LIQUIDITY_MONITOR!H29</f>
+        <v/>
+      </c>
+      <c r="I22" s="14">
+        <f>LIQUIDITY_MONITOR!I29</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Add comprehensive test suite for ExSim dashboards
- Create `run_full_suite.py` to orchestrate generation and validation.
- Update `self_test_dashboards.py` to include tests for Production Dashboard and fix CMO logic.
- Update `verify_integrity_suite.py` to include data integrity tests for Production Dashboard.
- Update `validate_dashboards.py` to cover Production Dashboard (handling folder typo).
- Fix minor bug in `generate_production_dashboard_zones.py`.
</commit_message>
<xml_diff>
--- a/CFO Dashboard/Finance_Dashboard_Final.xlsx
+++ b/CFO Dashboard/Finance_Dashboard_Final.xlsx
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>134500</v>
+        <v>56421</v>
       </c>
     </row>
     <row r="6">
@@ -899,7 +899,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>32749</v>
+        <v>28013</v>
       </c>
     </row>
     <row r="7">
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>134500</v>
+        <v>56421</v>
       </c>
       <c r="C9" s="8" t="inlineStr">
         <is>
@@ -1133,25 +1133,25 @@
         <v>0</v>
       </c>
       <c r="C19" s="11" t="n">
-        <v>221338</v>
+        <v>295885</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="11" t="n">
-        <v>74219</v>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="11" t="n">
-        <v>254176</v>
+      <c r="G19" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="H19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="11" t="n">
-        <v>202017</v>
+      <c r="I19" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1164,19 +1164,19 @@
         <v>0</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>-94059</v>
+        <v>-17468</v>
       </c>
       <c r="D20" s="11" t="n">
-        <v>-15792</v>
+        <v>-61630</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="11" t="n">
-        <v>-46165</v>
+        <v>-11620</v>
       </c>
       <c r="G20" s="11" t="n">
-        <v>-69087</v>
+        <v>-53250</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>0</v>
@@ -1544,7 +1544,7 @@
         </is>
       </c>
       <c r="B5" s="16" t="n">
-        <v>0.5911697410270922</v>
+        <v>0.593221527602339</v>
       </c>
     </row>
     <row r="6">
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="B6" s="16" t="n">
-        <v>0.03904386988246832</v>
+        <v>0.04422913950594023</v>
       </c>
     </row>
     <row r="9">
@@ -1593,10 +1593,10 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>952339</v>
+        <v>1183541</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>952339</v>
+        <v>1183541</v>
       </c>
       <c r="D11" s="18">
         <f>IF(B11&gt;0,(C11-B11)/B11,0)</f>
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>389345</v>
+        <v>481439</v>
       </c>
       <c r="C12" s="14">
         <f>C11*(1-$B$5)</f>
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>562994</v>
+        <v>702102</v>
       </c>
       <c r="C13" s="14">
         <f>C11-C12</f>
@@ -1663,10 +1663,10 @@
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>409407</v>
+        <v>361875</v>
       </c>
       <c r="C15" s="11" t="n">
-        <v>28960</v>
+        <v>43907</v>
       </c>
       <c r="D15" s="18">
         <f>IF(B15&gt;0,(C15-B15)/B15,0)</f>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="B17" s="19" t="n">
-        <v>37183</v>
+        <v>52347</v>
       </c>
       <c r="C17" s="15">
         <f>C13-C14-C15-C16</f>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>181621</v>
+        <v>183282</v>
       </c>
     </row>
     <row r="11">
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="B14" s="11" t="n">
-        <v>181621</v>
+        <v>183282</v>
       </c>
       <c r="C14" s="8" t="inlineStr">
         <is>

</xml_diff>